<commit_message>
Decided to change DB to GTEx+PAAD
</commit_message>
<xml_diff>
--- a/PAAD_Tables.xlsx
+++ b/PAAD_Tables.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,9 @@
       <c r="B11" s="1">
         <v>203</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>220</v>
+      </c>
       <c r="D11" s="1">
         <v>179</v>
       </c>
@@ -639,7 +641,9 @@
       <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>37</v>
+      </c>
       <c r="D12" s="1">
         <v>4</v>
       </c>
@@ -663,7 +667,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ref="D13" si="4">D11+D12</f>

</xml_diff>